<commit_message>
ASK-41 Remove MechanismType and Fix/adjust General information reader.
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmartktest_traject 12-2.xlsx
+++ b/benchmarktests/testdefinitions/Benchmartktest_traject 12-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C72F318-27C9-4FA6-B219-6DAF6DD66A33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7264ABC9-1032-4A3D-B53F-F5A7DE0B02D1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7665" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="10" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="28800" windowHeight="15435" tabRatio="653" firstSheet="1" activeTab="1" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="183">
   <si>
     <t>Vaknaam</t>
   </si>
@@ -587,6 +587,9 @@
   </si>
   <si>
     <t>Gecombineerd</t>
+  </si>
+  <si>
+    <t>Trajectlengte</t>
   </si>
 </sst>
 </file>
@@ -2456,7 +2459,7 @@
   </sheetPr>
   <dimension ref="B1:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:D106"/>
     </sheetView>
   </sheetViews>
@@ -6759,8 +6762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CBD9B7-2F4E-4E0F-B0DE-0C76068107FF}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6815,10 +6818,16 @@
         <v>1.111111111111111E-5</v>
       </c>
       <c r="F4" s="25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="9">
+        <v>20.93</v>
+      </c>
       <c r="D5" s="65" t="s">
         <v>42</v>
       </c>
@@ -6862,7 +6871,7 @@
         <v>45</v>
       </c>
       <c r="E8" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="27">
         <f>E7</f>

</xml_diff>